<commit_message>
BOM for V1 BGP
</commit_message>
<xml_diff>
--- a/BGP_V1/BOM.xlsx
+++ b/BGP_V1/BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="984" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="110">
   <si>
     <t xml:space="preserve">SHEET</t>
   </si>
@@ -211,28 +211,13 @@
     <t xml:space="preserve">TE CONNECTIVITY</t>
   </si>
   <si>
-    <t xml:space="preserve">Q</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2SK208-R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SC-59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOSHIBA</t>
-  </si>
-  <si>
     <t xml:space="preserve">U</t>
   </si>
   <si>
     <t xml:space="preserve">U1</t>
   </si>
   <si>
-    <t xml:space="preserve">ADA4077</t>
+    <t xml:space="preserve">MC33178</t>
   </si>
   <si>
     <t xml:space="preserve">SOIC-8</t>
@@ -343,28 +328,28 @@
     <t xml:space="preserve">L4</t>
   </si>
   <si>
+    <t xml:space="preserve">HPF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECH-U1H101JX5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECH-U1H272JX5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.7n</t>
+  </si>
+  <si>
     <t xml:space="preserve">OPA2170</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HPF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECH-U1H101JX5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100p</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECH-U1H272JX5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.7n</t>
   </si>
 </sst>
 </file>
@@ -480,19 +465,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J77"/>
+  <dimension ref="A1:J76"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.3"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.6836734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.9336734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -993,6 +978,9 @@
       <c r="G23" s="0" t="s">
         <v>62</v>
       </c>
+      <c r="H23" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="I23" s="0" t="n">
         <v>0.713</v>
       </c>
@@ -1007,7 +995,7 @@
       <c r="C24" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="0" t="s">
         <v>65</v>
       </c>
       <c r="E24" s="1" t="s">
@@ -1017,80 +1005,79 @@
       <c r="G24" s="0" t="s">
         <v>67</v>
       </c>
+      <c r="H24" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="I24" s="0" t="n">
-        <v>0.741</v>
+        <v>5.43</v>
       </c>
       <c r="J24" s="0" t="n">
-        <v>0.493</v>
+        <v>4.86</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
+      <c r="C25" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="D25" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="E25" s="0" t="s">
         <v>70</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="F25" s="0"/>
       <c r="G25" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="J25" s="0" t="n">
+        <v>1.54</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D26" s="0"/>
+      <c r="E26" s="0"/>
+      <c r="F26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="H25" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I25" s="0" t="n">
-        <v>5.43</v>
-      </c>
-      <c r="J25" s="0" t="n">
-        <v>4.86</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="0" t="s">
+      <c r="B27" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="0"/>
+      <c r="E27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="F26" s="0"/>
-      <c r="G26" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="H26" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I26" s="0" t="n">
-        <v>1.81</v>
-      </c>
-      <c r="J26" s="0" t="n">
-        <v>1.54</v>
+      <c r="H27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I27" s="3" t="n">
+        <v>0.069</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="C28" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D28" s="0"/>
       <c r="E28" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>78</v>
+        <v>19</v>
       </c>
       <c r="H28" s="0" t="n">
         <v>1</v>
@@ -1101,7 +1088,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D29" s="0"/>
       <c r="E29" s="1" t="s">
@@ -1119,7 +1106,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D30" s="0"/>
       <c r="E30" s="1" t="s">
@@ -1137,7 +1124,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D31" s="0"/>
       <c r="E31" s="1" t="s">
@@ -1155,7 +1142,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D32" s="0"/>
       <c r="E32" s="1" t="s">
@@ -1173,7 +1160,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D33" s="0"/>
       <c r="E33" s="1" t="s">
@@ -1191,7 +1178,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D34" s="0"/>
       <c r="E34" s="1" t="s">
@@ -1209,14 +1196,14 @@
     </row>
     <row r="35" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D35" s="0"/>
       <c r="E35" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="H35" s="0" t="n">
         <v>1</v>
@@ -1227,107 +1214,115 @@
     </row>
     <row r="36" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D36" s="0"/>
       <c r="E36" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I36" s="3" t="n">
+        <v>0.069</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="H37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I37" s="0" t="n">
+        <v>0.206</v>
+      </c>
+      <c r="J37" s="0" t="n">
+        <v>0.145</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C38" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H36" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I36" s="3" t="n">
-        <v>0.069</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D37" s="0"/>
-      <c r="E37" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H37" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I37" s="3" t="n">
-        <v>0.069</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="G38" s="0" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H38" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I38" s="0" t="n">
-        <v>0.206</v>
+        <v>1.18</v>
       </c>
       <c r="J38" s="0" t="n">
-        <v>0.145</v>
+        <v>0.671</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="H39" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I39" s="0" t="n">
-        <v>1.18</v>
+        <v>0.549</v>
       </c>
       <c r="J39" s="0" t="n">
-        <v>0.671</v>
+        <v>0.196</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="G40" s="0" t="s">
         <v>49</v>
@@ -1336,24 +1331,24 @@
         <v>1</v>
       </c>
       <c r="I40" s="0" t="n">
-        <v>0.549</v>
+        <v>0.206</v>
       </c>
       <c r="J40" s="0" t="n">
-        <v>0.196</v>
+        <v>0.145</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G41" s="0" t="s">
         <v>49</v>
@@ -1362,24 +1357,24 @@
         <v>1</v>
       </c>
       <c r="I41" s="0" t="n">
-        <v>0.206</v>
+        <v>0.823</v>
       </c>
       <c r="J41" s="0" t="n">
-        <v>0.145</v>
+        <v>0.494</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="G42" s="0" t="s">
         <v>49</v>
@@ -1388,15 +1383,15 @@
         <v>1</v>
       </c>
       <c r="I42" s="0" t="n">
-        <v>0.823</v>
+        <v>0.549</v>
       </c>
       <c r="J42" s="0" t="n">
-        <v>0.494</v>
+        <v>0.196</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="0" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>48</v>
@@ -1422,16 +1417,16 @@
     </row>
     <row r="44" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="0" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="G44" s="0" t="s">
         <v>49</v>
@@ -1440,73 +1435,71 @@
         <v>1</v>
       </c>
       <c r="I44" s="0" t="n">
-        <v>0.549</v>
+        <v>0.823</v>
       </c>
       <c r="J44" s="0" t="n">
-        <v>0.196</v>
+        <v>0.494</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="0" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>85</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>86</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H45" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I45" s="0" t="n">
-        <v>0.823</v>
+        <v>0.659</v>
       </c>
       <c r="J45" s="0" t="n">
-        <v>0.494</v>
+        <v>0.351</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="0" t="s">
+        <v>50</v>
+      </c>
       <c r="C46" s="0" t="s">
-        <v>89</v>
+        <v>51</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>91</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="F46" s="0"/>
       <c r="G46" s="0" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="H46" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I46" s="0" t="n">
-        <v>0.659</v>
+        <v>2.4</v>
       </c>
       <c r="J46" s="0" t="n">
-        <v>0.351</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
-        <v>50</v>
-      </c>
       <c r="C47" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>92</v>
+        <v>59</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>61</v>
@@ -1519,21 +1512,21 @@
         <v>1</v>
       </c>
       <c r="I47" s="0" t="n">
-        <v>2.4</v>
+        <v>0.713</v>
       </c>
       <c r="J47" s="0" t="n">
-        <v>2.1</v>
+        <v>0.631</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>60</v>
+        <v>88</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="F48" s="0"/>
       <c r="G48" s="0" t="s">
@@ -1543,18 +1536,18 @@
         <v>1</v>
       </c>
       <c r="I48" s="0" t="n">
-        <v>0.713</v>
+        <v>0.343</v>
       </c>
       <c r="J48" s="0" t="n">
-        <v>0.631</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="0" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>53</v>
@@ -1567,63 +1560,63 @@
         <v>1</v>
       </c>
       <c r="I49" s="0" t="n">
-        <v>0.343</v>
+        <v>0.137</v>
       </c>
       <c r="J49" s="0" t="n">
-        <v>0.265</v>
+        <v>0.071</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="0" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>53</v>
       </c>
       <c r="F50" s="0"/>
       <c r="G50" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H50" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I50" s="0" t="n">
-        <v>0.137</v>
-      </c>
-      <c r="J50" s="0" t="n">
-        <v>0.071</v>
+        <v>0.044</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="0" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>53</v>
       </c>
       <c r="F51" s="0"/>
       <c r="G51" s="0" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H51" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I51" s="0" t="n">
-        <v>0.044</v>
+        <v>0.343</v>
+      </c>
+      <c r="J51" s="0" t="n">
+        <v>0.265</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="0" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>53</v>
@@ -1636,63 +1629,63 @@
         <v>1</v>
       </c>
       <c r="I52" s="0" t="n">
-        <v>0.343</v>
+        <v>0.137</v>
       </c>
       <c r="J52" s="0" t="n">
-        <v>0.265</v>
+        <v>0.071</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="0" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>53</v>
       </c>
       <c r="F53" s="0"/>
       <c r="G53" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H53" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I53" s="0" t="n">
-        <v>0.137</v>
-      </c>
-      <c r="J53" s="0" t="n">
-        <v>0.071</v>
+        <v>0.044</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="0" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>53</v>
       </c>
       <c r="F54" s="0"/>
       <c r="G54" s="0" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H54" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I54" s="0" t="n">
-        <v>0.044</v>
+        <v>0.343</v>
+      </c>
+      <c r="J54" s="0" t="n">
+        <v>0.265</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="0" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>53</v>
@@ -1705,96 +1698,95 @@
         <v>1</v>
       </c>
       <c r="I55" s="0" t="n">
-        <v>0.343</v>
+        <v>0.137</v>
       </c>
       <c r="J55" s="0" t="n">
-        <v>0.265</v>
+        <v>0.071</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="0" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>53</v>
       </c>
       <c r="F56" s="0"/>
       <c r="G56" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H56" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I56" s="0" t="n">
-        <v>0.137</v>
-      </c>
-      <c r="J56" s="0" t="n">
-        <v>0.071</v>
+        <v>0.044</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="0" t="s">
+        <v>91</v>
+      </c>
       <c r="C57" s="0" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="F57" s="0"/>
-      <c r="G57" s="0" t="s">
-        <v>58</v>
-      </c>
       <c r="H57" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I57" s="0" t="n">
-        <v>0.044</v>
+        <v>0.274</v>
+      </c>
+      <c r="J57" s="0" t="n">
+        <v>0.246</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C58" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C58" s="0" t="s">
+      <c r="D58" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="E58" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="H58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I58" s="0" t="n">
+        <v>0.233</v>
+      </c>
+      <c r="J58" s="0" t="n">
+        <v>0.162</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C59" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="F58" s="0"/>
-      <c r="H58" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I58" s="0" t="n">
-        <v>0.274</v>
-      </c>
-      <c r="J58" s="0" t="n">
-        <v>0.246</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="C59" s="0" t="s">
-        <v>101</v>
-      </c>
       <c r="D59" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H59" s="0" t="n">
         <v>1</v>
@@ -1808,16 +1800,16 @@
     </row>
     <row r="60" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="0" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H60" s="0" t="n">
         <v>1</v>
@@ -1831,16 +1823,16 @@
     </row>
     <row r="61" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="0" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H61" s="0" t="n">
         <v>1</v>
@@ -1852,69 +1844,69 @@
         <v>0.162</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="0" t="s">
+        <v>63</v>
+      </c>
       <c r="C62" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D62" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F62" s="0"/>
+      <c r="G62" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="I62" s="0" t="n">
+        <v>2.52</v>
+      </c>
+      <c r="J62" s="0" t="n">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D63" s="0"/>
+      <c r="E63" s="0"/>
+      <c r="F63" s="0"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="E62" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F62" s="1" t="s">
+      <c r="B64" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D64" s="0"/>
+      <c r="E64" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F64" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H62" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I62" s="0" t="n">
-        <v>0.233</v>
-      </c>
-      <c r="J62" s="0" t="n">
-        <v>0.162</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="C63" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F63" s="0"/>
-      <c r="G63" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="I63" s="0" t="n">
-        <v>2.52</v>
-      </c>
-      <c r="J63" s="0" t="n">
-        <v>2.15</v>
+      <c r="H64" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I64" s="3" t="n">
+        <v>0.069</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="B65" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="C65" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D65" s="0"/>
       <c r="E65" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>109</v>
+        <v>17</v>
       </c>
       <c r="H65" s="0" t="n">
         <v>1</v>
@@ -1925,14 +1917,14 @@
     </row>
     <row r="66" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D66" s="0"/>
       <c r="E66" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H66" s="0" t="n">
         <v>1</v>
@@ -1943,14 +1935,14 @@
     </row>
     <row r="67" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D67" s="0"/>
       <c r="E67" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="H67" s="0" t="n">
         <v>1</v>
@@ -1961,14 +1953,14 @@
     </row>
     <row r="68" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D68" s="0"/>
       <c r="E68" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
       <c r="H68" s="0" t="n">
         <v>1</v>
@@ -1979,14 +1971,14 @@
     </row>
     <row r="69" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D69" s="0"/>
       <c r="E69" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>110</v>
+        <v>30</v>
       </c>
       <c r="H69" s="0" t="n">
         <v>1</v>
@@ -1996,88 +1988,112 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="0" t="s">
+        <v>31</v>
+      </c>
       <c r="C70" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D70" s="0"/>
+        <v>32</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="E70" s="1" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="H70" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I70" s="3" t="n">
-        <v>0.069</v>
+      <c r="I70" s="0" t="n">
+        <v>0.686</v>
+      </c>
+      <c r="J70" s="0" t="n">
+        <v>0.39</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="0" t="s">
-        <v>31</v>
-      </c>
       <c r="C71" s="0" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H71" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I71" s="0" t="n">
-        <v>0.686</v>
+        <v>0.768</v>
       </c>
       <c r="J71" s="0" t="n">
-        <v>0.39</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.442</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C72" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>113</v>
+        <v>48</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>114</v>
+        <v>40</v>
+      </c>
+      <c r="G72" s="0" t="s">
+        <v>49</v>
       </c>
       <c r="H72" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I72" s="0" t="n">
-        <v>0.768</v>
+        <v>0.549</v>
       </c>
       <c r="J72" s="0" t="n">
-        <v>0.442</v>
+        <v>0.196</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="0" t="s">
+        <v>50</v>
+      </c>
       <c r="C73" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D73" s="0"/>
-      <c r="E73" s="0"/>
+        <v>51</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G73" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="H73" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I73" s="0" t="n">
+        <v>0.343</v>
+      </c>
+      <c r="J73" s="0" t="n">
+        <v>0.265</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="0" t="s">
-        <v>50</v>
-      </c>
       <c r="C74" s="0" t="s">
         <v>51</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>53</v>
@@ -2089,10 +2105,10 @@
         <v>1</v>
       </c>
       <c r="I74" s="0" t="n">
-        <v>0.343</v>
+        <v>0.137</v>
       </c>
       <c r="J74" s="0" t="n">
-        <v>0.265</v>
+        <v>0.071</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2100,64 +2116,41 @@
         <v>51</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>53</v>
       </c>
       <c r="G75" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H75" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I75" s="0" t="n">
-        <v>0.137</v>
-      </c>
-      <c r="J75" s="0" t="n">
-        <v>0.071</v>
+        <v>0.044</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="0" t="s">
+        <v>63</v>
+      </c>
       <c r="C76" s="0" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="G76" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="H76" s="0" t="n">
-        <v>1</v>
+        <v>71</v>
       </c>
       <c r="I76" s="0" t="n">
-        <v>0.044</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="C77" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G77" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="I77" s="0" t="n">
         <v>2.52</v>
       </c>
-      <c r="J77" s="0" t="n">
+      <c r="J76" s="0" t="n">
         <v>2.15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Further component refinement in V1
</commit_message>
<xml_diff>
--- a/BGP_V1/BOM.xlsx
+++ b/BGP_V1/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="111">
   <si>
     <t xml:space="preserve">SHEET</t>
   </si>
@@ -272,6 +272,9 @@
   </si>
   <si>
     <t xml:space="preserve">C8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMCMA1C226MTRF</t>
   </si>
   <si>
     <t xml:space="preserve">C9</t>
@@ -467,17 +470,17 @@
   </sheetPr>
   <dimension ref="A1:J76"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G45" activeCellId="0" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="26.3214285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1420,16 +1423,16 @@
         <v>83</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>81</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="H44" s="0" t="n">
         <v>1</v>
@@ -1443,16 +1446,16 @@
     </row>
     <row r="45" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G45" s="0" t="s">
         <v>44</v>
@@ -1475,7 +1478,7 @@
         <v>51</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>61</v>
@@ -1520,7 +1523,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>52</v>
@@ -1544,7 +1547,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>56</v>
@@ -1568,7 +1571,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>57</v>
@@ -1589,7 +1592,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>52</v>
@@ -1613,7 +1616,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>56</v>
@@ -1637,7 +1640,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>57</v>
@@ -1658,7 +1661,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>52</v>
@@ -1682,7 +1685,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>56</v>
@@ -1706,7 +1709,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>57</v>
@@ -1727,16 +1730,16 @@
     </row>
     <row r="57" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F57" s="0"/>
       <c r="H57" s="0" t="n">
@@ -1751,19 +1754,19 @@
     </row>
     <row r="58" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H58" s="0" t="n">
         <v>1</v>
@@ -1777,16 +1780,16 @@
     </row>
     <row r="59" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H59" s="0" t="n">
         <v>1</v>
@@ -1800,16 +1803,16 @@
     </row>
     <row r="60" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H60" s="0" t="n">
         <v>1</v>
@@ -1823,16 +1826,16 @@
     </row>
     <row r="61" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H61" s="0" t="n">
         <v>1</v>
@@ -1875,7 +1878,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B64" s="0" t="s">
         <v>11</v>
@@ -1888,7 +1891,7 @@
         <v>13</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H64" s="0" t="n">
         <v>1</v>
@@ -1960,7 +1963,7 @@
         <v>13</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H68" s="0" t="n">
         <v>1</v>
@@ -1995,13 +1998,13 @@
         <v>32</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H70" s="0" t="n">
         <v>1</v>
@@ -2018,13 +2021,13 @@
         <v>37</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H71" s="0" t="n">
         <v>1</v>
@@ -2139,7 +2142,7 @@
         <v>64</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>66</v>

</xml_diff>

<commit_message>
V_0 Updates for caps, gerbers updated
</commit_message>
<xml_diff>
--- a/BGP_V1/BOM.xlsx
+++ b/BGP_V1/BOM.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="112">
   <si>
     <t xml:space="preserve">SHEET</t>
   </si>
@@ -329,6 +330,9 @@
   </si>
   <si>
     <t xml:space="preserve">L4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC7662BCOA713</t>
   </si>
   <si>
     <t xml:space="preserve">HPF</t>
@@ -370,7 +374,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -468,10 +471,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J76"/>
+  <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G45" activeCellId="0" sqref="G45"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B46" activeCellId="0" sqref="B46:J56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -515,7 +518,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>10</v>
       </c>
@@ -539,7 +542,7 @@
         <v>0.069</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
         <v>15</v>
@@ -558,7 +561,7 @@
         <v>0.069</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
@@ -576,7 +579,7 @@
         <v>0.069</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
@@ -594,7 +597,7 @@
         <v>0.069</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
@@ -612,7 +615,7 @@
         <v>0.069</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
@@ -630,7 +633,7 @@
         <v>0.069</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="2" t="s">
         <v>23</v>
       </c>
@@ -648,7 +651,7 @@
         <v>0.069</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="2" t="s">
         <v>24</v>
       </c>
@@ -666,7 +669,7 @@
         <v>0.069</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
         <v>26</v>
@@ -685,7 +688,7 @@
         <v>0.069</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="2" t="s">
         <v>27</v>
       </c>
@@ -703,7 +706,7 @@
         <v>0.069</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="2" t="s">
         <v>28</v>
       </c>
@@ -721,7 +724,7 @@
         <v>0.069</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="2" t="s">
         <v>29</v>
       </c>
@@ -1438,7 +1441,7 @@
         <v>1</v>
       </c>
       <c r="I44" s="0" t="n">
-        <v>0.823</v>
+        <v>0.37</v>
       </c>
       <c r="J44" s="0" t="n">
         <v>0.494</v>
@@ -1864,6 +1867,9 @@
       <c r="G62" s="0" t="s">
         <v>71</v>
       </c>
+      <c r="H62" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="I62" s="0" t="n">
         <v>2.52</v>
       </c>
@@ -1871,45 +1877,42 @@
         <v>2.15</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D63" s="0"/>
-      <c r="E63" s="0"/>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D63" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="F63" s="0"/>
+      <c r="H63" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I63" s="0" t="n">
+        <v>3.13</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="B64" s="0" t="s">
+      <c r="D64" s="0"/>
+      <c r="E64" s="0"/>
+      <c r="F64" s="0"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B65" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C64" s="0" t="s">
+      <c r="C65" s="0" t="s">
         <v>12</v>
-      </c>
-      <c r="D64" s="0"/>
-      <c r="E64" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H64" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I64" s="3" t="n">
-        <v>0.069</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C65" s="0" t="s">
-        <v>15</v>
       </c>
       <c r="D65" s="0"/>
       <c r="E65" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>17</v>
+        <v>105</v>
       </c>
       <c r="H65" s="0" t="n">
         <v>1</v>
@@ -1920,14 +1923,14 @@
     </row>
     <row r="66" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D66" s="0"/>
       <c r="E66" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H66" s="0" t="n">
         <v>1</v>
@@ -1938,14 +1941,14 @@
     </row>
     <row r="67" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="0" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D67" s="0"/>
       <c r="E67" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="H67" s="0" t="n">
         <v>1</v>
@@ -1956,14 +1959,14 @@
     </row>
     <row r="68" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D68" s="0"/>
       <c r="E68" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="H68" s="0" t="n">
         <v>1</v>
@@ -1974,129 +1977,124 @@
     </row>
     <row r="69" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D69" s="0"/>
       <c r="E69" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F69" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H69" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I69" s="3" t="n">
+        <v>0.069</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C70" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D70" s="0"/>
+      <c r="E70" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F70" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H69" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I69" s="3" t="n">
-        <v>0.069</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="0" t="s">
+      <c r="H70" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I70" s="3" t="n">
+        <v>0.069</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C70" s="0" t="s">
+      <c r="C71" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="D70" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F70" s="1" t="s">
+      <c r="D71" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="H70" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I70" s="0" t="n">
-        <v>0.686</v>
-      </c>
-      <c r="J70" s="0" t="n">
-        <v>0.39</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C71" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F71" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H71" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I71" s="0" t="n">
+        <v>0.686</v>
+      </c>
+      <c r="J71" s="0" t="n">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C72" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="H71" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I71" s="0" t="n">
-        <v>0.768</v>
-      </c>
-      <c r="J71" s="0" t="n">
-        <v>0.442</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C72" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F72" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H72" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I72" s="0" t="n">
+        <v>0.768</v>
+      </c>
+      <c r="J72" s="0" t="n">
+        <v>0.442</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C73" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F73" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G72" s="0" t="s">
+      <c r="G73" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="H72" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I72" s="0" t="n">
+      <c r="H73" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I73" s="0" t="n">
         <v>0.549</v>
       </c>
-      <c r="J72" s="0" t="n">
+      <c r="J73" s="0" t="n">
         <v>0.196</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="0" t="s">
+    <row r="74" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C73" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G73" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="H73" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I73" s="0" t="n">
-        <v>0.343</v>
-      </c>
-      <c r="J73" s="0" t="n">
-        <v>0.265</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="0" t="s">
         <v>51</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>53</v>
@@ -2108,10 +2106,10 @@
         <v>1</v>
       </c>
       <c r="I74" s="0" t="n">
-        <v>0.137</v>
+        <v>0.343</v>
       </c>
       <c r="J74" s="0" t="n">
-        <v>0.071</v>
+        <v>0.265</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2119,41 +2117,64 @@
         <v>51</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>53</v>
       </c>
       <c r="G75" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="H75" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I75" s="0" t="n">
+        <v>0.137</v>
+      </c>
+      <c r="J75" s="0" t="n">
+        <v>0.071</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C76" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G76" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="H75" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I75" s="0" t="n">
+      <c r="H76" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I76" s="0" t="n">
         <v>0.044</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="0" t="s">
+    <row r="77" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C76" s="0" t="s">
+      <c r="C77" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="D76" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E76" s="1" t="s">
+      <c r="D77" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E77" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G76" s="0" t="s">
+      <c r="G77" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="I76" s="0" t="n">
+      <c r="I77" s="0" t="n">
         <v>2.52</v>
       </c>
-      <c r="J76" s="0" t="n">
+      <c r="J77" s="0" t="n">
         <v>2.15</v>
       </c>
     </row>
@@ -2166,4 +2187,657 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I32"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G21" activeCellId="1" sqref="B46:J56 G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.1938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="n">
+        <v>0.069</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>0.069</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>0.069</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <v>0.069</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>0.069</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="n">
+        <v>0.069</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H7" s="3" t="n">
+        <v>0.069</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3" t="n">
+        <v>0.069</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H9" s="3" t="n">
+        <v>0.069</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="H10" s="3" t="n">
+        <v>0.069</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2"/>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H11" s="3" t="n">
+        <v>0.069</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>0.851</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>0.686</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>0.864</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>0.491</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>0.494</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>0.453</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>0.549</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>0.196</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>0.659</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>0.351</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>0.206</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>0.145</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>0.768</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>0.442</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>0.823</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>0.494</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>0.494</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>1.18</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>0.671</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>0.713</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>0.631</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>0.137</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <v>0.071</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>0.343</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>0.265</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>0.274</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>0.246</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <v>0.233</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <v>0.162</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <v>5.43</v>
+      </c>
+      <c r="I29" s="0" t="n">
+        <v>4.86</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <v>1.54</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H31" s="0" t="n">
+        <v>2.52</v>
+      </c>
+      <c r="I31" s="0" t="n">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H32" s="0" t="n">
+        <v>3.13</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>